<commit_message>
Minor bug fixes and clean-up
</commit_message>
<xml_diff>
--- a/scripts/plusarg_gen/tb_params.xlsx
+++ b/scripts/plusarg_gen/tb_params.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t xml:space="preserve">Parent name</t>
   </si>
@@ -84,16 +84,32 @@
     <t xml:space="preserve">amiq_dvcon_tb_seq0_0</t>
   </si>
   <si>
-    <t xml:space="preserve">red_field0_start_0</t>
+    <t xml:space="preserve">red_field0_constraints_range_start_0</t>
   </si>
   <si>
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">red_field0_end_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red_field0_weight_0</t>
+    <t xml:space="preserve">red_field0_constraints_range_end_0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">red_field0_constraints_range_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">weight_0</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">blue_pkt_nr</t>
@@ -117,22 +133,102 @@
     <t xml:space="preserve">amiq_dvcon_tb_seq0_2</t>
   </si>
   <si>
-    <t xml:space="preserve">purple_field0_start_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple_field0_end_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple_field0_weight_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple_field0_start_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple_field0_end_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple_field0_weight_1</t>
+    <t xml:space="preserve">purple_field0_constraints_range_start_0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">purple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_field0_constraints_range_end_0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">purple_field0_constraints_range_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">weight_0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">purple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_field0_constraints_range_start_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">purple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_field0_constraints_range_end_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">purple_field0_constraints_range_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">weight_1</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Object Type</t>
@@ -178,10 +274,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -206,7 +303,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF0064B3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Monospace"/>
       <family val="0"/>
       <charset val="1"/>
@@ -215,9 +318,14 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF0064B3"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -227,12 +335,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -269,8 +383,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,15 +412,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -315,7 +445,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -370,10 +500,10 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.26"/>
@@ -382,16 +512,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -451,8 +581,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="3"/>
+    </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2"/>
+      <c r="A34" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -473,31 +606,31 @@
   <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -505,10 +638,10 @@
       <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -519,7 +652,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -527,7 +660,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -535,7 +668,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -543,7 +676,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -554,10 +687,10 @@
       <c r="A7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -568,7 +701,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -576,7 +709,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -584,7 +717,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -595,10 +728,10 @@
       <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -609,7 +742,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -617,7 +750,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -625,7 +758,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -633,7 +766,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -641,7 +774,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -649,7 +782,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -657,7 +790,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -665,7 +798,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -673,121 +806,121 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="1"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="1"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="1"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="1"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="1"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="1"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="1"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="1"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="1"/>
+      <c r="B32" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="1"/>
+      <c r="C53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="1"/>
+      <c r="C54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="1"/>
+      <c r="C55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="1"/>
+      <c r="C56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="1"/>
+      <c r="C57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="1"/>
+      <c r="C58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="1"/>
+      <c r="C59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="1"/>
+      <c r="C60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="1"/>
+      <c r="C61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="1"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="1"/>
+      <c r="C83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="1"/>
+      <c r="C84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="1"/>
+      <c r="C85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="1"/>
+      <c r="C86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="1"/>
+      <c r="C87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="1"/>
+      <c r="C88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="1"/>
+      <c r="C89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="1"/>
+      <c r="C90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="1"/>
+      <c r="C91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="1"/>
+      <c r="B92" s="6"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C113" s="1"/>
+      <c r="C113" s="6"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="1"/>
+      <c r="C114" s="6"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="1"/>
+      <c r="C115" s="6"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="1"/>
+      <c r="C116" s="6"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="1"/>
+      <c r="C117" s="6"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="1"/>
+      <c r="C118" s="6"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="1"/>
+      <c r="C119" s="6"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="1"/>
+      <c r="C120" s="6"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="1"/>
+      <c r="C121" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -805,13 +938,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.91"/>
@@ -820,19 +953,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -840,13 +973,13 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -854,9 +987,9 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="D3" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="0" t="n">
@@ -864,9 +997,9 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="D4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="D4" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -874,7 +1007,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -882,7 +1015,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -890,7 +1023,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="0" t="n">
@@ -898,7 +1031,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -906,7 +1039,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="0" t="n">
@@ -914,7 +1047,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="0" t="n">
@@ -922,28 +1055,41 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="4"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="4"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="4"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>